<commit_message>
Enough bug fixing for passing tests
</commit_message>
<xml_diff>
--- a/inst/extdata/test_xtab2018.xlsx
+++ b/inst/extdata/test_xtab2018.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Bridgeport_1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Bridgeport_1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="TABLE1" vbProcedure="false">Bridgeport_1!$A$1</definedName>
@@ -404,56 +404,52 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -469,8 +465,114 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -490,7 +592,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="9.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="8.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="11.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="13.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="13.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="10.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="6.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="9.33"/>
@@ -557,7 +659,7 @@
       </c>
       <c r="T2" s="5"/>
     </row>
-    <row r="3" customFormat="false" ht="24.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4"/>
       <c r="B3" s="5" t="s">
         <v>7</v>
@@ -624,7 +726,7 @@
       <c r="B4" s="6"/>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
@@ -1016,7 +1118,7 @@
       </c>
       <c r="T13" s="5"/>
     </row>
-    <row r="14" customFormat="false" ht="24.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4"/>
       <c r="B14" s="5" t="s">
         <v>7</v>
@@ -1083,7 +1185,7 @@
       <c r="B15" s="6"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
         <v>27</v>
       </c>
@@ -1393,7 +1495,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
         <v>37</v>
       </c>
@@ -1563,7 +1665,7 @@
       <c r="S25" s="5"/>
       <c r="T25" s="5"/>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4"/>
       <c r="B26" s="5" t="s">
         <v>7</v>
@@ -1596,7 +1698,7 @@
       <c r="B27" s="6"/>
       <c r="C27" s="4"/>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
         <v>27</v>
       </c>
@@ -1777,7 +1879,7 @@
       </c>
       <c r="T36" s="5"/>
     </row>
-    <row r="37" customFormat="false" ht="24.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4"/>
       <c r="B37" s="5" t="s">
         <v>7</v>
@@ -1844,7 +1946,7 @@
       <c r="B38" s="6"/>
       <c r="C38" s="4"/>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
         <v>27</v>
       </c>
@@ -2204,7 +2306,7 @@
       </c>
       <c r="T46" s="5"/>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4"/>
       <c r="B47" s="5" t="s">
         <v>7</v>
@@ -2245,7 +2347,7 @@
       <c r="B48" s="6"/>
       <c r="C48" s="4"/>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="s">
         <v>27</v>
       </c>
@@ -2449,211 +2551,211 @@
       <c r="C58" s="9"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="10"/>
-      <c r="B59" s="10"/>
-      <c r="C59" s="11"/>
+      <c r="A59" s="3"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="10"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="10" t="s">
+      <c r="A60" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B60" s="10"/>
-      <c r="C60" s="11"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="10"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="10" t="s">
+      <c r="A61" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B61" s="10"/>
-      <c r="C61" s="12" t="n">
+      <c r="B61" s="3"/>
+      <c r="C61" s="11" t="n">
         <v>0.48</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="10" t="s">
+      <c r="A62" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B62" s="10"/>
-      <c r="C62" s="12" t="n">
+      <c r="B62" s="3"/>
+      <c r="C62" s="11" t="n">
         <v>0.52</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="10" t="s">
+      <c r="A63" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B63" s="10"/>
-      <c r="C63" s="11"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="10"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="10" t="s">
+      <c r="A64" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B64" s="10"/>
-      <c r="C64" s="12" t="n">
+      <c r="B64" s="3"/>
+      <c r="C64" s="11" t="n">
         <v>0.36</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="10" t="s">
+      <c r="A65" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B65" s="10"/>
-      <c r="C65" s="12" t="n">
+      <c r="B65" s="3"/>
+      <c r="C65" s="11" t="n">
         <v>0.24</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="10" t="s">
+      <c r="A66" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B66" s="10"/>
-      <c r="C66" s="12" t="n">
+      <c r="B66" s="3"/>
+      <c r="C66" s="11" t="n">
         <v>0.19</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="10" t="s">
+      <c r="A67" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B67" s="10"/>
-      <c r="C67" s="12" t="n">
+      <c r="B67" s="3"/>
+      <c r="C67" s="11" t="n">
         <v>0.16</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="10" t="s">
+      <c r="A68" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B68" s="10"/>
-      <c r="C68" s="12"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="11"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="10" t="s">
+      <c r="A69" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B69" s="10"/>
-      <c r="C69" s="12" t="n">
+      <c r="B69" s="3"/>
+      <c r="C69" s="11" t="n">
         <v>0.25</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="10" t="s">
+      <c r="A70" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B70" s="10"/>
-      <c r="C70" s="12" t="n">
+      <c r="B70" s="3"/>
+      <c r="C70" s="11" t="n">
         <v>0.33</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="10" t="s">
+      <c r="A71" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B71" s="10"/>
-      <c r="C71" s="12" t="n">
+      <c r="B71" s="3"/>
+      <c r="C71" s="11" t="n">
         <v>0.18</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="10" t="s">
+      <c r="A72" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B72" s="10"/>
-      <c r="C72" s="12" t="n">
+      <c r="B72" s="3"/>
+      <c r="C72" s="11" t="n">
         <v>0.22</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="10" t="s">
+      <c r="A73" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B73" s="10"/>
-      <c r="C73" s="11"/>
+      <c r="B73" s="3"/>
+      <c r="C73" s="10"/>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="10" t="s">
+      <c r="A74" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B74" s="10"/>
-      <c r="C74" s="12" t="n">
+      <c r="B74" s="3"/>
+      <c r="C74" s="11" t="n">
         <v>0.38</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="10" t="s">
+      <c r="A75" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B75" s="10"/>
-      <c r="C75" s="12" t="n">
+      <c r="B75" s="3"/>
+      <c r="C75" s="11" t="n">
         <v>0.34</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="10" t="s">
+      <c r="A76" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B76" s="10"/>
-      <c r="C76" s="12" t="n">
+      <c r="B76" s="3"/>
+      <c r="C76" s="11" t="n">
         <v>0.27</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="10" t="s">
+      <c r="A77" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B77" s="10"/>
-      <c r="C77" s="12"/>
+      <c r="B77" s="3"/>
+      <c r="C77" s="11"/>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="10" t="s">
+      <c r="A78" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B78" s="10"/>
-      <c r="C78" s="12" t="n">
+      <c r="B78" s="3"/>
+      <c r="C78" s="11" t="n">
         <v>0.4</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="10" t="s">
+      <c r="A79" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B79" s="10"/>
-      <c r="C79" s="12" t="n">
+      <c r="B79" s="3"/>
+      <c r="C79" s="11" t="n">
         <v>0.31</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="10" t="s">
+      <c r="A80" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B80" s="10"/>
-      <c r="C80" s="12" t="n">
+      <c r="B80" s="3"/>
+      <c r="C80" s="11" t="n">
         <v>0.17</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="10" t="s">
+      <c r="A81" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B81" s="10"/>
-      <c r="C81" s="12"/>
+      <c r="B81" s="3"/>
+      <c r="C81" s="11"/>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="10" t="s">
+      <c r="A82" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B82" s="10"/>
-      <c r="C82" s="12" t="n">
+      <c r="B82" s="3"/>
+      <c r="C82" s="11" t="n">
         <v>0.36</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="10" t="s">
+      <c r="A83" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B83" s="10"/>
-      <c r="C83" s="12" t="n">
+      <c r="B83" s="3"/>
+      <c r="C83" s="11" t="n">
         <v>0.62</v>
       </c>
     </row>
@@ -2700,7 +2802,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="0.879861111111111" bottom="0.529861111111111" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" scale="61" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="61" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;CDataHaven Community Wellbeing Survey
 conducted by the Siena College Research Institute

</xml_diff>